<commit_message>
Improved OOI assets file
</commit_message>
<xml_diff>
--- a/res/preload/r2_ioc/ooi_assets/OOIResourceMappings.xlsx
+++ b/res/preload/r2_ioc/ooi_assets/OOIResourceMappings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16380" tabRatio="669" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16380" tabRatio="669" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="7" r:id="rId1"/>
@@ -2226,7 +2226,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2247,6 +2247,22 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2265,9 +2281,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2275,7 +2313,29 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="24">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -2608,7 +2668,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -2792,7 +2854,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -4630,6 +4694,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4642,7 +4707,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K173"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G165" sqref="G165"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -10713,6 +10780,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -10725,14 +10793,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S87"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="66.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" customWidth="1"/>
+    <col min="17" max="17" width="46.5" customWidth="1"/>
+    <col min="18" max="18" width="13.5" customWidth="1"/>
+    <col min="19" max="19" width="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1">
@@ -15870,6 +15952,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -16293,7 +16376,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -16492,6 +16577,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -16504,7 +16590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>

</xml_diff>

<commit_message>
Updated OOI mapping spreadsheet
</commit_message>
<xml_diff>
--- a/res/preload/r2_ioc/ooi_assets/OOIResourceMappings.xlsx
+++ b/res/preload/r2_ioc/ooi_assets/OOIResourceMappings.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3967" uniqueCount="1118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3967" uniqueCount="1119">
   <si>
     <t>Platform Reference ID</t>
   </si>
@@ -3413,6 +3413,9 @@
   </si>
   <si>
     <t>Pull Mode</t>
+  </si>
+  <si>
+    <t>I1</t>
   </si>
 </sst>
 </file>
@@ -3532,7 +3535,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="866">
+  <cellStyleXfs count="872">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3559,6 +3562,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4455,7 +4464,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="866">
+  <cellStyles count="872">
     <cellStyle name="20% - Accent3" xfId="25" builtinId="38"/>
     <cellStyle name="40% - Accent2" xfId="24" builtinId="35"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -4889,6 +4898,9 @@
     <cellStyle name="Followed Hyperlink" xfId="861" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="863" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="865" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="867" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="869" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="871" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -5320,6 +5332,9 @@
     <cellStyle name="Hyperlink" xfId="860" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="862" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="864" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="866" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="868" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="870" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -9626,7 +9641,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11168,7 +11183,7 @@
         <v>196</v>
       </c>
       <c r="G34" s="8" t="str">
-        <f t="shared" ref="G34:G65" si="1">E34 &amp; IF(ISBLANK(F34),""," " &amp; F34)</f>
+        <f t="shared" ref="G34:G59" si="1">E34 &amp; IF(ISBLANK(F34),""," " &amp; F34)</f>
         <v>Global Irminger Sea Subsurface</v>
       </c>
     </row>
@@ -11813,8 +11828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W195"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12458,7 +12473,7 @@
       <c r="R11" s="17"/>
       <c r="S11" s="17"/>
       <c r="U11" s="3" t="s">
-        <v>843</v>
+        <v>1118</v>
       </c>
       <c r="V11" t="s">
         <v>1079</v>
@@ -13080,7 +13095,7 @@
       <c r="R22" s="17"/>
       <c r="S22" s="17"/>
       <c r="U22" s="3" t="s">
-        <v>843</v>
+        <v>1118</v>
       </c>
       <c r="V22" t="s">
         <v>1080</v>
@@ -21055,7 +21070,7 @@
       <c r="R174" s="16"/>
       <c r="S174" s="16"/>
       <c r="U174" s="3" t="s">
-        <v>843</v>
+        <v>1118</v>
       </c>
       <c r="V174" t="s">
         <v>1091</v>
@@ -21184,8 +21199,8 @@
       <c r="P176" t="s">
         <v>635</v>
       </c>
-      <c r="U176" s="26" t="s">
-        <v>843</v>
+      <c r="U176" s="3" t="s">
+        <v>1118</v>
       </c>
       <c r="V176" s="2" t="s">
         <v>1081</v>
@@ -21439,7 +21454,7 @@
       <c r="R180" s="16"/>
       <c r="S180" s="16"/>
       <c r="U180" s="3" t="s">
-        <v>843</v>
+        <v>1118</v>
       </c>
       <c r="V180" t="s">
         <v>1083</v>
@@ -21631,7 +21646,7 @@
         <v>635</v>
       </c>
       <c r="U183" s="3" t="s">
-        <v>843</v>
+        <v>1118</v>
       </c>
       <c r="V183" t="s">
         <v>1087</v>
@@ -22406,8 +22421,8 @@
         <v>635</v>
       </c>
       <c r="T195" s="3"/>
-      <c r="U195" s="26" t="s">
-        <v>843</v>
+      <c r="U195" s="3" t="s">
+        <v>1118</v>
       </c>
       <c r="V195" t="s">
         <v>1091</v>

</xml_diff>

<commit_message>
Refined PlatformSite hierarchy and added alt_resource_type attribute
</commit_message>
<xml_diff>
--- a/res/preload/r2_ioc/ooi_assets/OOIResourceMappings.xlsx
+++ b/res/preload/r2_ioc/ooi_assets/OOIResourceMappings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22380" tabRatio="669" activeTab="4"/>
+    <workbookView xWindow="560" yWindow="0" windowWidth="38400" windowHeight="22400" tabRatio="669" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="MIOs" sheetId="14" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3967" uniqueCount="1119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3973" uniqueCount="1125">
   <si>
     <t>Platform Reference ID</t>
   </si>
@@ -3416,6 +3416,24 @@
   </si>
   <si>
     <t>I1</t>
+  </si>
+  <si>
+    <t>lat_north</t>
+  </si>
+  <si>
+    <t>lat_south</t>
+  </si>
+  <si>
+    <t>lon_east</t>
+  </si>
+  <si>
+    <t>lon_west</t>
+  </si>
+  <si>
+    <t>depth_min</t>
+  </si>
+  <si>
+    <t>depth_max</t>
   </si>
 </sst>
 </file>
@@ -3535,7 +3553,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="872">
+  <cellStyleXfs count="880">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4408,8 +4426,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4463,8 +4489,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="872">
+  <cellStyles count="880">
     <cellStyle name="20% - Accent3" xfId="25" builtinId="38"/>
     <cellStyle name="40% - Accent2" xfId="24" builtinId="35"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -4901,6 +4930,10 @@
     <cellStyle name="Followed Hyperlink" xfId="867" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="869" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="871" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="873" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="875" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="877" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="879" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -5335,6 +5368,10 @@
     <cellStyle name="Hyperlink" xfId="866" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="868" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="870" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="872" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="874" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="876" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="878" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -10320,10 +10357,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10334,9 +10371,10 @@
     <col min="5" max="5" width="28.5" style="8" customWidth="1"/>
     <col min="6" max="6" width="28.33203125" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="45.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:14" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>99</v>
       </c>
@@ -10358,11 +10396,29 @@
       <c r="G1" s="9" t="s">
         <v>631</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="33" t="s">
+        <v>1119</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>1120</v>
+      </c>
+      <c r="J1" s="33" t="s">
+        <v>1121</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>1122</v>
+      </c>
+      <c r="L1" s="33" t="s">
+        <v>1123</v>
+      </c>
+      <c r="M1" s="33" t="s">
+        <v>1124</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>111</v>
       </c>
@@ -10387,7 +10443,7 @@
         <v>Coastal Endurance Oregon Inshore</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>120</v>
       </c>
@@ -10412,7 +10468,7 @@
         <v>Coastal Endurance Oregon Inshore</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>124</v>
       </c>
@@ -10437,7 +10493,7 @@
         <v>Coastal Endurance Oregon Shelf</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>131</v>
       </c>
@@ -10462,7 +10518,7 @@
         <v>Coastal Endurance Oregon Shelf</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>137</v>
       </c>
@@ -10487,7 +10543,7 @@
         <v>Coastal Endurance Oregon Shelf</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>139</v>
       </c>
@@ -10512,7 +10568,7 @@
         <v>Coastal Endurance Oregon Offshore</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>277</v>
       </c>
@@ -10537,7 +10593,7 @@
         <v>Coastal Endurance Oregon Offshore</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>142</v>
       </c>
@@ -10562,7 +10618,7 @@
         <v>Coastal Endurance Oregon Offshore</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>234</v>
       </c>
@@ -10586,8 +10642,26 @@
         <f t="shared" si="0"/>
         <v>Coastal Endurance Mobile Zone</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="H10" s="11">
+        <v>47</v>
+      </c>
+      <c r="I10" s="11">
+        <v>44.64</v>
+      </c>
+      <c r="J10" s="11">
+        <v>-124.95</v>
+      </c>
+      <c r="K10" s="11">
+        <v>124.1</v>
+      </c>
+      <c r="L10" s="11">
+        <v>0</v>
+      </c>
+      <c r="M10" s="11">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>144</v>
       </c>
@@ -10612,7 +10686,7 @@
         <v>Coastal Endurance Washington Inshore</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>147</v>
       </c>
@@ -10637,7 +10711,7 @@
         <v>Coastal Endurance Washington Inshore</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>149</v>
       </c>
@@ -10662,7 +10736,7 @@
         <v>Coastal Endurance Washington Shelf</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>155</v>
       </c>
@@ -10687,7 +10761,7 @@
         <v>Coastal Endurance Washington Shelf</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>157</v>
       </c>
@@ -10712,7 +10786,7 @@
         <v>Coastal Endurance Washington Offshore</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>162</v>
       </c>
@@ -10737,7 +10811,7 @@
         <v>Coastal Endurance Washington Offshore</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>164</v>
       </c>
@@ -10762,7 +10836,7 @@
         <v>Coastal Pioneer Central</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>168</v>
       </c>
@@ -10787,7 +10861,7 @@
         <v>Coastal Pioneer Central</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>170</v>
       </c>
@@ -10812,7 +10886,7 @@
         <v>Coastal Pioneer Central Inshore</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>172</v>
       </c>
@@ -10837,7 +10911,7 @@
         <v>Coastal Pioneer Central Offshore</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>174</v>
       </c>
@@ -10862,7 +10936,7 @@
         <v>Coastal Pioneer Upstream Inshore</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>177</v>
       </c>
@@ -10887,7 +10961,7 @@
         <v>Coastal Pioneer Upstream Offshore</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>180</v>
       </c>
@@ -10912,7 +10986,7 @@
         <v>Coastal Pioneer Inshore</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>183</v>
       </c>
@@ -10937,7 +11011,7 @@
         <v>Coastal Pioneer Inshore</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>185</v>
       </c>
@@ -10962,7 +11036,7 @@
         <v>Coastal Pioneer Offshore</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>188</v>
       </c>
@@ -10987,7 +11061,7 @@
         <v>Coastal Pioneer Offshore</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>243</v>
       </c>
@@ -11011,8 +11085,26 @@
         <f t="shared" si="0"/>
         <v>Coastal Pioneer Mobile Zone</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27" s="11">
+        <v>40.166666669999998</v>
+      </c>
+      <c r="I27" s="11">
+        <v>39.908333329999998</v>
+      </c>
+      <c r="J27" s="11">
+        <v>-70.791666669999998</v>
+      </c>
+      <c r="K27" s="11">
+        <v>-70.683333329999996</v>
+      </c>
+      <c r="L27" s="11">
+        <v>0</v>
+      </c>
+      <c r="M27" s="11">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>190</v>
       </c>
@@ -11037,7 +11129,7 @@
         <v>Global Argentine Basin Surface</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>194</v>
       </c>
@@ -11062,7 +11154,7 @@
         <v>Global Argentine Basin Subsurface</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>201</v>
       </c>
@@ -11087,7 +11179,7 @@
         <v>Global Argentine Basin Mesoscale Flanking A</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>206</v>
       </c>
@@ -11112,7 +11204,7 @@
         <v>Global Argentine Basin Mesoscale Flanking B</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>255</v>
       </c>
@@ -11136,8 +11228,26 @@
         <f t="shared" si="0"/>
         <v>Global Argentine Basin Mobile Zone</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="H32" s="11">
+        <v>-42.507300000000001</v>
+      </c>
+      <c r="I32" s="11">
+        <v>-42.990600000000001</v>
+      </c>
+      <c r="J32" s="11">
+        <v>-42.890500000000003</v>
+      </c>
+      <c r="K32" s="11">
+        <v>-42.130299999999998</v>
+      </c>
+      <c r="L32" s="11">
+        <v>0</v>
+      </c>
+      <c r="M32" s="11">
+        <v>5200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" t="s">
         <v>208</v>
       </c>
@@ -11162,7 +11272,7 @@
         <v>Global Irminger Sea Surface</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:14">
       <c r="A34" t="s">
         <v>211</v>
       </c>
@@ -11187,7 +11297,7 @@
         <v>Global Irminger Sea Subsurface</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
         <v>213</v>
       </c>
@@ -11212,7 +11322,7 @@
         <v>Global Irminger Sea Mesoscale Flanking A</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:14">
       <c r="A36" t="s">
         <v>215</v>
       </c>
@@ -11237,7 +11347,7 @@
         <v>Global Irminger Sea Mesoscale Flanking B</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:14">
       <c r="A37" t="s">
         <v>263</v>
       </c>
@@ -11261,8 +11371,26 @@
         <f t="shared" si="1"/>
         <v>Global Irminger Sea Mobile Zone</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="H37" s="11">
+        <v>60.613599999999998</v>
+      </c>
+      <c r="I37" s="11">
+        <v>60.458199999999998</v>
+      </c>
+      <c r="J37" s="11">
+        <v>-38.4407</v>
+      </c>
+      <c r="K37" s="11">
+        <v>-38.075499999999998</v>
+      </c>
+      <c r="L37" s="11">
+        <v>0</v>
+      </c>
+      <c r="M37" s="11">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
         <v>217</v>
       </c>
@@ -11287,7 +11415,7 @@
         <v>Global Station Papa Subsurface</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:14">
       <c r="A39" t="s">
         <v>220</v>
       </c>
@@ -11312,7 +11440,7 @@
         <v>Global Station Papa Mesoscale Flanking A</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:14">
       <c r="A40" t="s">
         <v>222</v>
       </c>
@@ -11337,7 +11465,7 @@
         <v>Global Station Papa Mesoscale Flanking B</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:14">
       <c r="A41" t="s">
         <v>268</v>
       </c>
@@ -11361,8 +11489,26 @@
         <f t="shared" si="1"/>
         <v>Global Station Papa Mobile Zone</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="H41" s="11">
+        <v>50.467599999999997</v>
+      </c>
+      <c r="I41" s="11">
+        <v>50.125</v>
+      </c>
+      <c r="J41" s="11">
+        <v>-144.7131</v>
+      </c>
+      <c r="K41" s="11">
+        <v>-144.2097</v>
+      </c>
+      <c r="L41" s="11">
+        <v>0</v>
+      </c>
+      <c r="M41" s="11">
+        <v>4250</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
       <c r="A42" t="s">
         <v>224</v>
       </c>
@@ -11387,7 +11533,7 @@
         <v>Global Southern Ocean Surface</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:14">
       <c r="A43" t="s">
         <v>227</v>
       </c>
@@ -11412,7 +11558,7 @@
         <v>Global Southern Ocean Subsurface</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:14">
       <c r="A44" t="s">
         <v>229</v>
       </c>
@@ -11437,7 +11583,7 @@
         <v>Global Southern Ocean Mesoscale Flanking A</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:14">
       <c r="A45" t="s">
         <v>231</v>
       </c>
@@ -11462,7 +11608,7 @@
         <v>Global Southern Ocean Mesoscale Flanking B</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:14">
       <c r="A46" t="s">
         <v>273</v>
       </c>
@@ -11486,8 +11632,26 @@
         <f t="shared" si="1"/>
         <v>Global Southern Ocean Mobile Zone</v>
       </c>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="H46" s="11">
+        <v>-54.081400000000002</v>
+      </c>
+      <c r="I46" s="11">
+        <v>-54.470399999999998</v>
+      </c>
+      <c r="J46" s="11">
+        <v>-89.665199999999999</v>
+      </c>
+      <c r="K46" s="11">
+        <v>-88.894000000000005</v>
+      </c>
+      <c r="L46" s="11">
+        <v>0</v>
+      </c>
+      <c r="M46" s="11">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
       <c r="A47" t="s">
         <v>1088</v>
       </c>
@@ -11508,11 +11672,29 @@
         <f t="shared" si="1"/>
         <v>Regional Shore Pacific City</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H47" s="11">
+        <v>45.214548999999998</v>
+      </c>
+      <c r="I47" s="11">
+        <v>45.214548999999998</v>
+      </c>
+      <c r="J47" s="11">
+        <v>-123.96768299999999</v>
+      </c>
+      <c r="K47" s="11">
+        <v>-123.96768299999999</v>
+      </c>
+      <c r="L47" s="11">
+        <v>0</v>
+      </c>
+      <c r="M47" s="11">
+        <v>0</v>
+      </c>
+      <c r="N47" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:14">
       <c r="A48" t="s">
         <v>285</v>
       </c>
@@ -11537,7 +11719,7 @@
         <v>Regional Hydrate Ridge Slope Base</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:14">
       <c r="A49" t="s">
         <v>290</v>
       </c>
@@ -11562,7 +11744,7 @@
         <v>Regional Hydrate Ridge Slope Base</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:14">
       <c r="A50" t="s">
         <v>294</v>
       </c>
@@ -11587,7 +11769,7 @@
         <v>Regional Hydrate Ridge Southern Summit</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:14">
       <c r="A51" t="s">
         <v>296</v>
       </c>
@@ -11612,7 +11794,7 @@
         <v>Regional Hydrate Ridge Southern Summit</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:14">
       <c r="A52" t="s">
         <v>298</v>
       </c>
@@ -11637,7 +11819,7 @@
         <v>Regional Axial Ashes</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:14">
       <c r="A53" t="s">
         <v>302</v>
       </c>
@@ -11662,7 +11844,7 @@
         <v>Regional Axial Base</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:14">
       <c r="A54" t="s">
         <v>304</v>
       </c>
@@ -11687,7 +11869,7 @@
         <v>Regional Axial Base</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:14">
       <c r="A55" t="s">
         <v>306</v>
       </c>
@@ -11712,7 +11894,7 @@
         <v>Regional Axial Central Caldera</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:14">
       <c r="A56" t="s">
         <v>308</v>
       </c>
@@ -11737,7 +11919,7 @@
         <v>Regional Axial Eastern Caldera</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:14">
       <c r="A57" t="s">
         <v>310</v>
       </c>
@@ -11762,7 +11944,7 @@
         <v>Regional Axial International District</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:14">
       <c r="A58" t="s">
         <v>312</v>
       </c>
@@ -11787,7 +11969,7 @@
         <v>Regional Axial International District</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:14">
       <c r="A59" t="s">
         <v>717</v>
       </c>
@@ -11806,7 +11988,25 @@
         <f t="shared" si="1"/>
         <v>Regional Mid Plate</v>
       </c>
-      <c r="H59" t="s">
+      <c r="H59" s="11">
+        <v>45.755560000000003</v>
+      </c>
+      <c r="I59" s="11">
+        <v>45.755560000000003</v>
+      </c>
+      <c r="J59" s="11">
+        <v>-127.27861</v>
+      </c>
+      <c r="K59" s="11">
+        <v>-127.27861</v>
+      </c>
+      <c r="L59" s="11">
+        <v>2820</v>
+      </c>
+      <c r="M59" s="11">
+        <v>2820</v>
+      </c>
+      <c r="N59" t="s">
         <v>716</v>
       </c>
     </row>
@@ -11828,8 +12028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>